<commit_message>
Actualización del cronogrma, cierre de tarea
</commit_message>
<xml_diff>
--- a/Cronograma_TFG.xlsx
+++ b/Cronograma_TFG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorena\Desktop\TFG_Lorena\Trabajo-Fin-de-Grado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E4F621-B67E-445F-A065-CA8104D390FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D15BA89-6983-4A96-A8FB-2645BC664AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -737,7 +737,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -890,6 +890,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -917,7 +918,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1214,8 +1215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="Z12" sqref="Z12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1227,30 +1228,30 @@
   <sheetData>
     <row r="1" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C2" s="88" t="s">
+      <c r="C2" s="89" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="89"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="93" t="s">
+      <c r="D2" s="90"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="94"/>
-      <c r="H2" s="94"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="88" t="s">
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="89" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="88" t="s">
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="91"/>
+      <c r="O2" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="P2" s="89"/>
-      <c r="Q2" s="89"/>
-      <c r="R2" s="90"/>
+      <c r="P2" s="90"/>
+      <c r="Q2" s="90"/>
+      <c r="R2" s="91"/>
       <c r="S2" s="62" t="s">
         <v>27</v>
       </c>
@@ -1316,7 +1317,7 @@
       <c r="T3" s="2"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A4" s="91" t="s">
+      <c r="A4" s="92" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="76" t="s">
@@ -1341,7 +1342,7 @@
       <c r="S4" s="63"/>
     </row>
     <row r="5" spans="1:20" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="96"/>
+      <c r="A5" s="97"/>
       <c r="B5" s="77" t="s">
         <v>1</v>
       </c>
@@ -1364,7 +1365,7 @@
       <c r="S5" s="64"/>
     </row>
     <row r="6" spans="1:20" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="92"/>
+      <c r="A6" s="93"/>
       <c r="B6" s="78" t="s">
         <v>2</v>
       </c>
@@ -1412,7 +1413,7 @@
       <c r="S7" s="66"/>
     </row>
     <row r="8" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="91" t="s">
+      <c r="A8" s="92" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="69" t="s">
@@ -1437,7 +1438,7 @@
       <c r="S8" s="66"/>
     </row>
     <row r="9" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="92"/>
+      <c r="A9" s="93"/>
       <c r="B9" s="69" t="s">
         <v>44</v>
       </c>
@@ -1447,7 +1448,7 @@
       <c r="F9" s="37"/>
       <c r="G9" s="29"/>
       <c r="H9" s="87"/>
-      <c r="I9" s="97"/>
+      <c r="I9" s="88"/>
       <c r="J9" s="37"/>
       <c r="K9" s="29"/>
       <c r="L9" s="29"/>
@@ -1460,7 +1461,7 @@
       <c r="S9" s="66"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A10" s="91" t="s">
+      <c r="A10" s="92" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="76" t="s">
@@ -1485,7 +1486,7 @@
       <c r="S10" s="63"/>
     </row>
     <row r="11" spans="1:20" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="96"/>
+      <c r="A11" s="97"/>
       <c r="B11" s="77" t="s">
         <v>8</v>
       </c>
@@ -1508,7 +1509,7 @@
       <c r="S11" s="64"/>
     </row>
     <row r="12" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="92"/>
+      <c r="A12" s="93"/>
       <c r="B12" s="78" t="s">
         <v>9</v>
       </c>
@@ -1531,7 +1532,7 @@
       <c r="S12" s="65"/>
     </row>
     <row r="13" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="91" t="s">
+      <c r="A13" s="92" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="76" t="s">
@@ -1543,7 +1544,7 @@
       <c r="F13" s="40"/>
       <c r="G13" s="80"/>
       <c r="H13" s="80"/>
-      <c r="I13" s="11"/>
+      <c r="I13" s="98"/>
       <c r="J13" s="32"/>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
@@ -1556,7 +1557,7 @@
       <c r="S13" s="63"/>
     </row>
     <row r="14" spans="1:20" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="96"/>
+      <c r="A14" s="97"/>
       <c r="B14" s="77" t="s">
         <v>11</v>
       </c>
@@ -1579,7 +1580,7 @@
       <c r="S14" s="64"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A15" s="96"/>
+      <c r="A15" s="97"/>
       <c r="B15" s="77" t="s">
         <v>12</v>
       </c>
@@ -1602,7 +1603,7 @@
       <c r="S15" s="64"/>
     </row>
     <row r="16" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="92"/>
+      <c r="A16" s="93"/>
       <c r="B16" s="78" t="s">
         <v>13</v>
       </c>
@@ -1625,7 +1626,7 @@
       <c r="S16" s="65"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A17" s="91" t="s">
+      <c r="A17" s="92" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="76" t="s">
@@ -1650,7 +1651,7 @@
       <c r="S17" s="63"/>
     </row>
     <row r="18" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="92"/>
+      <c r="A18" s="93"/>
       <c r="B18" s="78" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Coreccion de algun error y actualizacion de el cronograma
</commit_message>
<xml_diff>
--- a/Cronograma_TFG.xlsx
+++ b/Cronograma_TFG.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorena\Desktop\TFG_Lorena\Trabajo-Fin-de-Grado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C33E3A5-495F-46A5-99F7-118125B92483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD029C2-678F-4E98-8379-15B02BEBF801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,18 +51,12 @@
     <t>DESARROLLO DEL ALGORITMO</t>
   </si>
   <si>
-    <t>Implementar y probar el algoritmo</t>
-  </si>
-  <si>
     <t>DESARROLLO DE LA APLICACIÓN SHINY</t>
   </si>
   <si>
     <t>Diseñar la estructura y funcionalidad de la APP</t>
   </si>
   <si>
-    <t>Integrar el algoritmo con la aplicación</t>
-  </si>
-  <si>
     <t>Realizar pruebas y corregir errores</t>
   </si>
   <si>
@@ -160,6 +154,12 @@
   </si>
   <si>
     <t>Definir los modelos a desarrollar</t>
+  </si>
+  <si>
+    <t>Integración de los resultados obtenidos</t>
+  </si>
+  <si>
+    <t>Creación de mapas resultantes</t>
   </si>
 </sst>
 </file>
@@ -287,7 +287,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -739,11 +739,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -842,7 +894,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
@@ -899,6 +950,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -926,8 +979,14 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1225,7 +1284,7 @@
   <dimension ref="A1:T26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="AA9" sqref="AA9"/>
+      <selection activeCell="X27" sqref="X27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1237,100 +1296,100 @@
   <sheetData>
     <row r="1" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C2" s="91" t="s">
+      <c r="C2" s="92" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="93"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="97" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="92"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="96" t="s">
+      <c r="K2" s="93"/>
+      <c r="L2" s="93"/>
+      <c r="M2" s="93"/>
+      <c r="N2" s="94"/>
+      <c r="O2" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="91" t="s">
+      <c r="P2" s="93"/>
+      <c r="Q2" s="93"/>
+      <c r="R2" s="94"/>
+      <c r="S2" s="61" t="s">
         <v>24</v>
-      </c>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="93"/>
-      <c r="O2" s="91" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="92"/>
-      <c r="Q2" s="92"/>
-      <c r="R2" s="93"/>
-      <c r="S2" s="62" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="69" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="70" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="71" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="69" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="72" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="73" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="69" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="72" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" s="72" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="72" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="73" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="69" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" s="72" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3" s="72" t="s">
+        <v>37</v>
+      </c>
+      <c r="R3" s="73" t="s">
+        <v>38</v>
+      </c>
+      <c r="S3" s="74" t="s">
+        <v>39</v>
+      </c>
+      <c r="T3" s="2"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A4" s="95" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="75" t="s">
         <v>19</v>
-      </c>
-      <c r="C3" s="70" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="71" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="72" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="70" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="73" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="73" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="74" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" s="70" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="73" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" s="73" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" s="73" t="s">
-        <v>35</v>
-      </c>
-      <c r="N3" s="74" t="s">
-        <v>36</v>
-      </c>
-      <c r="O3" s="70" t="s">
-        <v>37</v>
-      </c>
-      <c r="P3" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q3" s="73" t="s">
-        <v>39</v>
-      </c>
-      <c r="R3" s="74" t="s">
-        <v>40</v>
-      </c>
-      <c r="S3" s="75" t="s">
-        <v>41</v>
-      </c>
-      <c r="T3" s="2"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A4" s="94" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="76" t="s">
-        <v>21</v>
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="17"/>
@@ -1348,11 +1407,11 @@
       <c r="P4" s="20"/>
       <c r="Q4" s="20"/>
       <c r="R4" s="21"/>
-      <c r="S4" s="63"/>
+      <c r="S4" s="62"/>
     </row>
     <row r="5" spans="1:20" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="99"/>
-      <c r="B5" s="77" t="s">
+      <c r="A5" s="100"/>
+      <c r="B5" s="76" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="22"/>
@@ -1371,11 +1430,11 @@
       <c r="P5" s="14"/>
       <c r="Q5" s="14"/>
       <c r="R5" s="23"/>
-      <c r="S5" s="64"/>
+      <c r="S5" s="63"/>
     </row>
     <row r="6" spans="1:20" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="95"/>
-      <c r="B6" s="78" t="s">
+      <c r="A6" s="96"/>
+      <c r="B6" s="77" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="24"/>
@@ -1394,20 +1453,20 @@
       <c r="P6" s="27"/>
       <c r="Q6" s="27"/>
       <c r="R6" s="28"/>
-      <c r="S6" s="65"/>
+      <c r="S6" s="64"/>
     </row>
     <row r="7" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="69" t="s">
+      <c r="B7" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="82"/>
-      <c r="D7" s="83"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="81"/>
+      <c r="G7" s="81"/>
       <c r="H7" s="29"/>
       <c r="I7" s="45"/>
       <c r="J7" s="37"/>
@@ -1419,21 +1478,21 @@
       <c r="P7" s="30"/>
       <c r="Q7" s="30"/>
       <c r="R7" s="31"/>
-      <c r="S7" s="66"/>
+      <c r="S7" s="65"/>
     </row>
     <row r="8" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="94" t="s">
+      <c r="A8" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="69" t="s">
+      <c r="B8" s="68" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="37"/>
       <c r="D8" s="29"/>
-      <c r="E8" s="85"/>
-      <c r="F8" s="85"/>
-      <c r="G8" s="86"/>
-      <c r="H8" s="90"/>
+      <c r="E8" s="84"/>
+      <c r="F8" s="84"/>
+      <c r="G8" s="85"/>
+      <c r="H8" s="89"/>
       <c r="I8" s="45"/>
       <c r="J8" s="37"/>
       <c r="K8" s="29"/>
@@ -1444,20 +1503,20 @@
       <c r="P8" s="30"/>
       <c r="Q8" s="30"/>
       <c r="R8" s="31"/>
-      <c r="S8" s="66"/>
+      <c r="S8" s="65"/>
     </row>
     <row r="9" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="95"/>
-      <c r="B9" s="69" t="s">
-        <v>42</v>
+      <c r="A9" s="96"/>
+      <c r="B9" s="68" t="s">
+        <v>40</v>
       </c>
       <c r="C9" s="37"/>
       <c r="D9" s="29"/>
       <c r="E9" s="37"/>
       <c r="F9" s="37"/>
       <c r="G9" s="29"/>
-      <c r="H9" s="87"/>
-      <c r="I9" s="88"/>
+      <c r="H9" s="86"/>
+      <c r="I9" s="87"/>
       <c r="J9" s="37"/>
       <c r="K9" s="29"/>
       <c r="L9" s="29"/>
@@ -1467,22 +1526,22 @@
       <c r="P9" s="30"/>
       <c r="Q9" s="30"/>
       <c r="R9" s="31"/>
-      <c r="S9" s="66"/>
+      <c r="S9" s="65"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A10" s="94" t="s">
+      <c r="A10" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="76" t="s">
-        <v>44</v>
+      <c r="B10" s="75" t="s">
+        <v>42</v>
       </c>
       <c r="C10" s="32"/>
       <c r="D10" s="10"/>
       <c r="E10" s="21"/>
       <c r="F10" s="32"/>
       <c r="G10" s="10"/>
-      <c r="H10" s="79"/>
-      <c r="I10" s="101"/>
+      <c r="H10" s="78"/>
+      <c r="I10" s="91"/>
       <c r="J10" s="32"/>
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
@@ -1492,12 +1551,12 @@
       <c r="P10" s="20"/>
       <c r="Q10" s="20"/>
       <c r="R10" s="21"/>
-      <c r="S10" s="63"/>
+      <c r="S10" s="62"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A11" s="99"/>
-      <c r="B11" s="77" t="s">
-        <v>43</v>
+      <c r="A11" s="100"/>
+      <c r="B11" s="76" t="s">
+        <v>41</v>
       </c>
       <c r="C11" s="33"/>
       <c r="D11" s="13"/>
@@ -1505,141 +1564,141 @@
       <c r="F11" s="33"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
-      <c r="I11" s="100"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="47"/>
-      <c r="O11" s="33"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="23"/>
-      <c r="S11" s="64"/>
-    </row>
-    <row r="12" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="95"/>
-      <c r="B12" s="78" t="s">
+      <c r="I11" s="90"/>
+      <c r="J11" s="101"/>
+      <c r="K11" s="102"/>
+      <c r="L11" s="102"/>
+      <c r="M11" s="102"/>
+      <c r="N11" s="90"/>
+      <c r="O11" s="105"/>
+      <c r="P11" s="107"/>
+      <c r="Q11" s="107"/>
+      <c r="R11" s="106"/>
+      <c r="S11" s="108"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A12" s="100"/>
+      <c r="B12" s="76" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="33"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="47"/>
+      <c r="O12" s="33"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="23"/>
+      <c r="S12" s="63"/>
+    </row>
+    <row r="13" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="96"/>
+      <c r="B13" s="77" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="34"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="35"/>
+      <c r="N13" s="48"/>
+      <c r="O13" s="34"/>
+      <c r="P13" s="27"/>
+      <c r="Q13" s="27"/>
+      <c r="R13" s="28"/>
+      <c r="S13" s="64"/>
+    </row>
+    <row r="14" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="95" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="34"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="36"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="35"/>
-      <c r="N12" s="48"/>
-      <c r="O12" s="34"/>
-      <c r="P12" s="27"/>
-      <c r="Q12" s="27"/>
-      <c r="R12" s="28"/>
-      <c r="S12" s="65"/>
-    </row>
-    <row r="13" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="94" t="s">
+      <c r="B14" s="75" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="32"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="79"/>
+      <c r="H14" s="79"/>
+      <c r="I14" s="88"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="62"/>
+    </row>
+    <row r="15" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="100"/>
+      <c r="B15" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="76" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="80"/>
-      <c r="H13" s="80"/>
-      <c r="I13" s="89"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="32"/>
-      <c r="P13" s="20"/>
-      <c r="Q13" s="20"/>
-      <c r="R13" s="21"/>
-      <c r="S13" s="63"/>
-    </row>
-    <row r="14" spans="1:20" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="99"/>
-      <c r="B14" s="77" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="81"/>
-      <c r="H14" s="81"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="47"/>
-      <c r="O14" s="33"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="23"/>
-      <c r="S14" s="64"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A15" s="99"/>
-      <c r="B15" s="77" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="38"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="54"/>
-      <c r="O15" s="57"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="80"/>
+      <c r="H15" s="80"/>
+      <c r="I15" s="103"/>
+      <c r="J15" s="104"/>
+      <c r="K15" s="80"/>
+      <c r="L15" s="80"/>
+      <c r="M15" s="80"/>
+      <c r="N15" s="103"/>
+      <c r="O15" s="33"/>
       <c r="P15" s="14"/>
       <c r="Q15" s="14"/>
       <c r="R15" s="23"/>
-      <c r="S15" s="64"/>
+      <c r="S15" s="63"/>
     </row>
     <row r="16" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="95"/>
-      <c r="B16" s="78" t="s">
+      <c r="A16" s="100"/>
+      <c r="B16" s="76" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="38"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="54"/>
+      <c r="O16" s="57"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="23"/>
+      <c r="S16" s="63"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A17" s="95" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="75" t="s">
         <v>12</v>
-      </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="27"/>
-      <c r="N16" s="28"/>
-      <c r="O16" s="58"/>
-      <c r="P16" s="36"/>
-      <c r="Q16" s="27"/>
-      <c r="R16" s="28"/>
-      <c r="S16" s="65"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A17" s="94" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="76" t="s">
-        <v>14</v>
       </c>
       <c r="C17" s="40"/>
       <c r="D17" s="6"/>
@@ -1657,12 +1716,12 @@
       <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
       <c r="R17" s="46"/>
-      <c r="S17" s="63"/>
+      <c r="S17" s="62"/>
     </row>
     <row r="18" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="95"/>
-      <c r="B18" s="78" t="s">
-        <v>15</v>
+      <c r="A18" s="96"/>
+      <c r="B18" s="77" t="s">
+        <v>13</v>
       </c>
       <c r="C18" s="39"/>
       <c r="D18" s="27"/>
@@ -1679,15 +1738,15 @@
       <c r="O18" s="39"/>
       <c r="P18" s="27"/>
       <c r="Q18" s="36"/>
-      <c r="R18" s="59"/>
-      <c r="S18" s="65"/>
+      <c r="R18" s="58"/>
+      <c r="S18" s="64"/>
     </row>
     <row r="19" spans="1:19" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="68" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="69" t="s">
-        <v>17</v>
+      <c r="A19" s="67" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="68" t="s">
+        <v>15</v>
       </c>
       <c r="C19" s="49"/>
       <c r="D19" s="50"/>
@@ -1703,9 +1762,9 @@
       <c r="N19" s="51"/>
       <c r="O19" s="49"/>
       <c r="P19" s="50"/>
-      <c r="Q19" s="60"/>
-      <c r="R19" s="61"/>
-      <c r="S19" s="67"/>
+      <c r="Q19" s="59"/>
+      <c r="R19" s="60"/>
+      <c r="S19" s="66"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A20" s="7"/>
@@ -1729,10 +1788,10 @@
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A10:A13"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="J2:N2"/>
-    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="A14:A16"/>
     <mergeCell ref="A8:A9"/>
   </mergeCells>
   <pageMargins left="0.11811023622047245" right="0.11811023622047245" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>